<commit_message>
Ajout schémas mapping 33cf523b0ab00096696278d58d4c1c8eb8410e1a
</commit_message>
<xml_diff>
--- a/ig/amelioration-mapping/StructureDefinition-ror-location.xlsx
+++ b/ig/amelioration-mapping/StructureDefinition-ror-location.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-12T09:47:28+00:00</t>
+    <t>2024-01-19T15:31:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2698,7 +2698,7 @@
 </t>
   </si>
   <si>
-    <t>systemeGeodesique (CoordonneeGeographique) : Permet de signaler si les informations des coordonnées géographiques sont issues d'un mode de production qui assure un certain niveau de fiabilité</t>
+    <t>coordonneesFiables (CoordonneeGeographique) : Permet de signaler si les informations des coordonnées géographiques sont issues d'un mode de production qui assure un certain niveau de fiabilité</t>
   </si>
   <si>
     <t>Extension créée dans le cadre du ROR pour signaler si les informations des coordonnées géographiques sont issues d'un mode de production qui assure un certain niveau de fiabilité</t>

</xml_diff>